<commit_message>
I changed test data sheet.
</commit_message>
<xml_diff>
--- a/github_acceptance_test.xlsx
+++ b/github_acceptance_test.xlsx
@@ -588,27 +588,15 @@
     <t>Itleialanieladf laijleklafioqeenljlaflfadfjleriaeroaljvndfanj oillkearnanfafaf oadfoioyjxvljcvljaldjfaofsajflkjkvklyjvjia ojadfjaodfasflvnaf aoifaodrjaerljaldflvna adflaf adlfaiflkfaowejdfkasdkfjlvnandsaf jlijlajdfv fafafaljfalfafa oqoqoeoqjefasknlvnafdasf</t>
   </si>
   <si>
-    <t>pelda@sagem.com</t>
-  </si>
-  <si>
     <t>A rendszer hibaüzenetet dob fel, nem fogadja el a beírt adatot</t>
   </si>
   <si>
-    <t>Itleialanieladf laijleklafioqeenljlaflfadfjleriaeroaljvndfanj oillkearnanfafaf oadfoioyjxvljcvljaldjfaofsajflkjkvklyjvjia ojadfjaodfasflvnaf aoifaodrjaerljaldflvna adflaf adlfaiflkfaowejdfkasdkfjlvnandsaf jlijlajdfv fafafaljfalfafa oqoqoeoqjefasknlvnafdasf@sagemsagemsagemsagemsagemsagemsagemsagemsagemsagemsagemsagem.com</t>
-  </si>
-  <si>
     <t>p@s.co</t>
   </si>
   <si>
     <t>p@s.c</t>
   </si>
   <si>
-    <t>Itleialanieladf laijleklafioqeenljlaflfadfjleriaeroaljvndfanj oillkearnanfafaf oadfoioyjxvljcvljaldjfaofsajflkjkvklyjvjia ojadfjaodfasflvnaf aoifaodrjaerljaldflvna adflaf adlfaiflkfaowejdfkasdkfjlvnandsaf jlijlajdfv fafafaljfalfafa oqoqoeoqjefasknlvnaf@sagemsagemsagemsagemsagemsagemsagemsagemsagemsagemsagemsagem.com</t>
-  </si>
-  <si>
-    <t>p@sagem.com</t>
-  </si>
-  <si>
     <t>@</t>
   </si>
   <si>
@@ -639,19 +627,7 @@
     <t>Tóth-Béla-Sára</t>
   </si>
   <si>
-    <t>PO@SAGEM.COM</t>
-  </si>
-  <si>
-    <t>!#$%&amp;'*+-/=?^_{|}~@sagem.com</t>
-  </si>
-  <si>
-    <t>””:; &lt;&gt;@sagem.com</t>
-  </si>
-  <si>
     <t>Ellenőrizd, hogy az E-mail mező ””:; &lt;&gt; speciális karaktereket nem fogad el.</t>
-  </si>
-  <si>
-    <t>tóthbéla@sagem.com</t>
   </si>
   <si>
     <t>TzFaB2</t>
@@ -1035,6 +1011,30 @@
   </si>
   <si>
     <t>Ez a dokumentum tartalmazza a "Hipotetikus regisztrációs felület" rendszer "Új felhasználó regisztráció" moduljának elfogadási tesztjének tervezetét, követelményeit és folyamatábráját. A követelmények nyomonkövethetőségét a Requirement Traceability Matrix-szal biztosítjuk. A teszt esetek lefuttatásához teszt adatokat terveztünk, amelyeknek előállítását/rendelkezésre állását a teszt környezetben biztosítani szükséges.</t>
+  </si>
+  <si>
+    <t>!#$%&amp;'*+-/=?^_{|}~@info.com</t>
+  </si>
+  <si>
+    <t>””:; &lt;&gt;@info.com</t>
+  </si>
+  <si>
+    <t>tóthbéla@info.com</t>
+  </si>
+  <si>
+    <t>pelda@info.com</t>
+  </si>
+  <si>
+    <t>Itleialanieladf laijleklafioqeenljlaflfadfjleriaeroaljvndfanj oillkearnanfafaf oadfoioyjxvljcvljaldjfaofsajflkjkvklyjvjia ojadfjaodfasflvnaf aoifaodrjaerljaldflvna adflaf adlfaiflkfaowejdfkasdkfjlvnandsaf jlijlajdfv fafafaljfalfafa oqoqoeoqjefasknlvnaf@infoinfoinfoinfoinfoinfoinfoinfoinfoinfoinfoinfo.com</t>
+  </si>
+  <si>
+    <t>p@info.com</t>
+  </si>
+  <si>
+    <t>Itleialanieladf laijleklafioqeenljlaflfadfjleriaeroaljvndfanj oillkearnanfafaf oadfoioyjxvljcvljaldjfaofsajflkjkvklyjvjia ojadfjaodfasflvnaf aoifaodrjaerljaldflvna adflaf adlfaiflkfaowejdfkasdkfjlvnandsaf jlijlajdfv fafafaljfalfafa oqoqoeoqjefasknlvnafdasf@infoinfoinfoinfoinfoinfoinfoinfoinfoinfoinfoinfo.com</t>
+  </si>
+  <si>
+    <t>PO@info.COM</t>
   </si>
 </sst>
 </file>
@@ -1610,7 +1610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1624,7 +1624,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="21" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
@@ -1632,31 +1632,31 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="C3" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="C4" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="C5" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="C6" s="17">
         <v>44335</v>
@@ -1665,18 +1665,18 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C7" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D8" s="13"/>
     </row>
@@ -1688,14 +1688,14 @@
     </row>
     <row r="11" spans="2:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="22" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
     </row>
     <row r="12" spans="2:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="23" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
@@ -1716,30 +1716,30 @@
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="C17" s="19">
         <v>44335</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -1809,7 +1809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A59"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A48" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -1817,7 +1817,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -1847,7 +1847,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1931,7 +1931,7 @@
         <v>R001</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>14</v>
@@ -1959,7 +1959,7 @@
         <v>R001</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>14</v>
@@ -1987,7 +1987,7 @@
         <v>R001</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>15</v>
@@ -2015,7 +2015,7 @@
         <v>R001</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>15</v>
@@ -2043,7 +2043,7 @@
         <v>R001</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>15</v>
@@ -2071,7 +2071,7 @@
         <v>R001</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>16</v>
@@ -2099,7 +2099,7 @@
         <v>R001</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>16</v>
@@ -2127,7 +2127,7 @@
         <v>R001</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>16</v>
@@ -2155,7 +2155,7 @@
         <v>R001</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>16</v>
@@ -2183,7 +2183,7 @@
         <v>R001</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>16</v>
@@ -2211,7 +2211,7 @@
         <v>R001</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>16</v>
@@ -2239,7 +2239,7 @@
         <v>R001</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>31</v>
@@ -2267,7 +2267,7 @@
         <v>R001</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>31</v>
@@ -2295,7 +2295,7 @@
         <v>R001</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>31</v>
@@ -2323,7 +2323,7 @@
         <v>R001</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>31</v>
@@ -2351,7 +2351,7 @@
         <v>R001</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>31</v>
@@ -2379,7 +2379,7 @@
         <v>R001</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>31</v>
@@ -2407,7 +2407,7 @@
         <v>R001</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>33</v>
@@ -2435,7 +2435,7 @@
         <v>R001</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>33</v>
@@ -2463,7 +2463,7 @@
         <v>R001</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>35</v>
@@ -2491,7 +2491,7 @@
         <v>R001</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>35</v>
@@ -2519,7 +2519,7 @@
         <v>R001</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>35</v>
@@ -2547,7 +2547,7 @@
         <v>R001</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>35</v>
@@ -2575,7 +2575,7 @@
         <v>R002</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>43</v>
@@ -2603,7 +2603,7 @@
         <v>R002</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>43</v>
@@ -2920,7 +2920,7 @@
         <v>158</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>149</v>
@@ -2932,7 +2932,7 @@
         <v>151</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>152</v>
@@ -2970,10 +2970,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>174</v>
@@ -2999,10 +2999,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>174</v>
@@ -3028,7 +3028,7 @@
         <v>5</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>176</v>
@@ -3054,10 +3054,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>174</v>
@@ -3083,7 +3083,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>180</v>
@@ -3109,10 +3109,10 @@
         <v>5</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>174</v>
@@ -3138,10 +3138,10 @@
         <v>5</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>174</v>
@@ -3167,10 +3167,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>174</v>
@@ -3196,10 +3196,10 @@
         <v>1</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>174</v>
@@ -3225,10 +3225,10 @@
         <v>2</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>174</v>
@@ -3254,10 +3254,10 @@
         <v>2</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>174</v>
@@ -3283,10 +3283,10 @@
         <v>5</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>174</v>
@@ -3312,10 +3312,10 @@
         <v>5</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>174</v>
@@ -3341,10 +3341,10 @@
         <v>2</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>174</v>
@@ -3370,10 +3370,10 @@
         <v>2</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>174</v>
@@ -3390,7 +3390,7 @@
         <v>95</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>159</v>
@@ -3399,10 +3399,10 @@
         <v>2</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>174</v>
@@ -3428,10 +3428,10 @@
         <v>5</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>174</v>
@@ -3457,13 +3457,13 @@
         <v>1</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>175</v>
@@ -3486,10 +3486,10 @@
         <v>1</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>174</v>
@@ -3515,13 +3515,13 @@
         <v>2</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3541,13 +3541,13 @@
         <v>2</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3567,13 +3567,13 @@
         <v>3</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3593,13 +3593,13 @@
         <v>1</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="J24" s="8" t="s">
         <v>175</v>
@@ -3610,7 +3610,7 @@
         <v>137</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>103</v>
@@ -3625,13 +3625,13 @@
         <v>1</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3639,7 +3639,7 @@
         <v>138</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>104</v>
@@ -3648,19 +3648,19 @@
         <v>45</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3677,7 +3677,7 @@
         <v>3</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3694,7 +3694,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3711,7 +3711,7 @@
         <v>3</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3728,7 +3728,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -3745,7 +3745,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -3753,7 +3753,7 @@
         <v>144</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>110</v>
@@ -3762,22 +3762,22 @@
         <v>61</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="F32">
         <v>1</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3785,7 +3785,7 @@
         <v>145</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>111</v>
@@ -3794,22 +3794,22 @@
         <v>59</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3817,7 +3817,7 @@
         <v>146</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>112</v>
@@ -3826,22 +3826,22 @@
         <v>62</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -3849,7 +3849,7 @@
         <v>147</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>113</v>
@@ -3858,22 +3858,22 @@
         <v>59</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="F35">
         <v>1</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3890,8 +3890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3915,7 +3915,7 @@
         <v>155</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4007,7 +4007,7 @@
         <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C8" t="s">
         <v>160</v>
@@ -4022,7 +4022,7 @@
         <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C9" t="s">
         <v>161</v>
@@ -4037,7 +4037,7 @@
         <v>115</v>
       </c>
       <c r="B10" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C10" t="s">
         <v>162</v>
@@ -4052,7 +4052,7 @@
         <v>115</v>
       </c>
       <c r="B11" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C11" t="s">
         <v>163</v>
@@ -4067,7 +4067,7 @@
         <v>115</v>
       </c>
       <c r="B12" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C12" t="s">
         <v>164</v>
@@ -4082,7 +4082,7 @@
         <v>115</v>
       </c>
       <c r="B13" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C13" t="s">
         <v>165</v>
@@ -4097,7 +4097,7 @@
         <v>117</v>
       </c>
       <c r="B14" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C14" t="s">
         <v>178</v>
@@ -4112,7 +4112,7 @@
         <v>117</v>
       </c>
       <c r="B15" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C15" t="s">
         <v>179</v>
@@ -4127,13 +4127,13 @@
         <v>119</v>
       </c>
       <c r="B16" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C16" t="s">
         <v>182</v>
       </c>
       <c r="D16" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4141,13 +4141,13 @@
         <v>119</v>
       </c>
       <c r="B17" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C17" t="s">
         <v>183</v>
       </c>
       <c r="D17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4155,13 +4155,13 @@
         <v>120</v>
       </c>
       <c r="B18" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>184</v>
+        <v>316</v>
       </c>
       <c r="D18" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -4169,13 +4169,13 @@
         <v>120</v>
       </c>
       <c r="B19" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C19" t="s">
-        <v>189</v>
+        <v>317</v>
       </c>
       <c r="D19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4183,13 +4183,13 @@
         <v>121</v>
       </c>
       <c r="B20" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>190</v>
+        <v>318</v>
       </c>
       <c r="D20" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -4197,13 +4197,13 @@
         <v>121</v>
       </c>
       <c r="B21" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D21" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -4211,13 +4211,13 @@
         <v>122</v>
       </c>
       <c r="B22" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C22" t="s">
-        <v>186</v>
+        <v>319</v>
       </c>
       <c r="D22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -4225,13 +4225,13 @@
         <v>122</v>
       </c>
       <c r="B23" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -4239,13 +4239,13 @@
         <v>122</v>
       </c>
       <c r="B24" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C24" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -4253,13 +4253,13 @@
         <v>123</v>
       </c>
       <c r="B25" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="C25" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -4267,13 +4267,13 @@
         <v>123</v>
       </c>
       <c r="B26" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C26" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D26" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -4281,13 +4281,13 @@
         <v>124</v>
       </c>
       <c r="B27" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C27" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4295,13 +4295,13 @@
         <v>124</v>
       </c>
       <c r="B28" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="C28" t="s">
+        <v>190</v>
+      </c>
+      <c r="D28" t="s">
         <v>194</v>
-      </c>
-      <c r="D28" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -4309,13 +4309,13 @@
         <v>125</v>
       </c>
       <c r="B29" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C29" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D29" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4323,13 +4323,13 @@
         <v>125</v>
       </c>
       <c r="B30" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C30" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D30" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4337,13 +4337,13 @@
         <v>126</v>
       </c>
       <c r="B31" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C31" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D31" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -4351,13 +4351,13 @@
         <v>126</v>
       </c>
       <c r="B32" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C32" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D32" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -4365,13 +4365,13 @@
         <v>127</v>
       </c>
       <c r="B33" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>201</v>
+        <v>320</v>
       </c>
       <c r="D33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -4379,13 +4379,13 @@
         <v>128</v>
       </c>
       <c r="B34" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="C34" t="s">
-        <v>202</v>
+        <v>313</v>
       </c>
       <c r="D34" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -4393,13 +4393,13 @@
         <v>129</v>
       </c>
       <c r="B35" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C35" t="s">
-        <v>203</v>
+        <v>314</v>
       </c>
       <c r="D35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -4407,13 +4407,13 @@
         <v>130</v>
       </c>
       <c r="B36" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>205</v>
+        <v>315</v>
       </c>
       <c r="D36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -4421,16 +4421,16 @@
         <v>131</v>
       </c>
       <c r="B37" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="C37" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D37" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E37" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -4438,16 +4438,16 @@
         <v>131</v>
       </c>
       <c r="B38" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="C38" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D38" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E38" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -4455,13 +4455,13 @@
         <v>132</v>
       </c>
       <c r="B39" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="C39" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D39" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -4469,16 +4469,16 @@
         <v>136</v>
       </c>
       <c r="B40" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C40" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D40" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E40" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -4486,16 +4486,16 @@
         <v>136</v>
       </c>
       <c r="B41" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="C41" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="D41" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E41" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -4503,16 +4503,16 @@
         <v>136</v>
       </c>
       <c r="B42" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="C42" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="D42" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E42" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -4520,25 +4520,25 @@
         <v>136</v>
       </c>
       <c r="B43" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="C43" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="D43" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="E43" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C18" r:id="rId1"/>
-    <hyperlink ref="C20" r:id="rId2"/>
+    <hyperlink ref="C20" r:id="rId2" display="p@sagem.com"/>
     <hyperlink ref="C21" r:id="rId3"/>
     <hyperlink ref="C23" r:id="rId4"/>
-    <hyperlink ref="C33" r:id="rId5"/>
+    <hyperlink ref="C33" r:id="rId5" display="PO@SAGEM.COM"/>
     <hyperlink ref="C36" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4567,7 +4567,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>21</v>
@@ -4673,16 +4673,16 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B9" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="C9" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="D9" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>